<commit_message>
added Expt 3, showing that MLEs are perfect with huge k
</commit_message>
<xml_diff>
--- a/*2021-5-9 nonaffirm MLEs on Sherlock/Results/*agg_rounded_annotated.xlsx
+++ b/*2021-5-9 nonaffirm MLEs on Sherlock/Results/*agg_rounded_annotated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmathur/Dropbox/Personal computer/Independent studies/2021/Sensitivity analysis for p-hacking (SAPH)/Code (git)/*2021-5-9 nonaffirm MLEs on Sherlock/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E09C0B2-9BC1-F746-BD21-D5B4476DC703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D947CBE9-D108-B045-A00D-AB675DA1355D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="1300" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2540" yWindow="1560" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agg_rounded" sheetId="1" r:id="rId1"/>
@@ -1098,8 +1098,8 @@
   <dimension ref="A1:AT32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D25" sqref="D25"/>
+      <pane xSplit="5" topLeftCell="AE1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF8" sqref="AF8:AG25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
separate sim code archives from living versions of Sherlock code
</commit_message>
<xml_diff>
--- a/*2021-5-9 nonaffirm MLEs on Sherlock/Results/*agg_rounded_annotated.xlsx
+++ b/*2021-5-9 nonaffirm MLEs on Sherlock/Results/*agg_rounded_annotated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmathur/Dropbox/Personal computer/Independent studies/2021/Sensitivity analysis for p-hacking (SAPH)/Code (git)/*2021-5-9 nonaffirm MLEs on Sherlock/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D947CBE9-D108-B045-A00D-AB675DA1355D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3358BB3-0C60-9643-8CD4-A4B1C7717A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="1560" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="1840" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agg_rounded" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>T2</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Blue background = same parameters as local.R experiment #1, except there I had Mu = 1 instead of Mu = 0.1 and had an enormous k</t>
+  </si>
+  <si>
+    <t>Grey background = same parameters (except maybe k) as experiments #3.1-3.3 in local.R</t>
   </si>
 </sst>
 </file>
@@ -361,7 +364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +568,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -726,7 +735,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
@@ -740,6 +749,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1095,11 +1106,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT32"/>
+  <dimension ref="A1:AT33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="AE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF8" sqref="AF8:AG25"/>
+      <pane xSplit="5" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D33" sqref="B33:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3554,131 +3565,131 @@
         <v>8.2100000000000009</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>0.25</v>
-      </c>
-      <c r="B20">
-        <v>0.25</v>
-      </c>
-      <c r="C20">
+    <row r="20" spans="1:46" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="B20" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="C20" s="13">
         <v>1</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
+      <c r="D20" s="13">
+        <v>0</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0</v>
+      </c>
+      <c r="F20" s="13">
         <v>0.1</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="13">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="13">
         <v>0.27</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="13">
         <v>0.94</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="13">
         <v>0.3</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="13">
         <v>0.1</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="13">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="13">
         <v>0.27</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="13">
         <v>0.94</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="13">
         <v>0.3</v>
       </c>
-      <c r="P20" s="1">
+      <c r="P20" s="13">
         <v>0.12</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="13">
         <v>-0.23</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="13">
         <v>0.47</v>
       </c>
-      <c r="S20" s="1">
+      <c r="S20" s="13">
         <v>0.94</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="13">
         <v>0.51</v>
       </c>
-      <c r="U20">
+      <c r="U20" s="13">
         <v>84.61</v>
       </c>
-      <c r="V20">
+      <c r="V20" s="13">
         <v>84.61</v>
       </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
-      <c r="X20">
+      <c r="W20" s="13">
+        <v>0</v>
+      </c>
+      <c r="X20" s="13">
         <v>-0.28999999999999998</v>
       </c>
-      <c r="Y20">
+      <c r="Y20" s="13">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="Z20">
+      <c r="Z20" s="13">
         <v>-0.28000000000000003</v>
       </c>
-      <c r="AB20">
+      <c r="AB20" s="13">
         <v>1.91</v>
       </c>
-      <c r="AC20">
+      <c r="AC20" s="13">
         <v>1.91</v>
       </c>
-      <c r="AD20">
+      <c r="AD20" s="13">
         <v>1.91</v>
       </c>
-      <c r="AF20" s="10">
+      <c r="AF20" s="14">
         <v>0.2</v>
       </c>
-      <c r="AG20" s="10">
+      <c r="AG20" s="14">
         <v>0.24</v>
       </c>
-      <c r="AH20">
+      <c r="AH20" s="13">
         <v>-0.47</v>
       </c>
-      <c r="AI20">
+      <c r="AI20" s="13">
         <v>0.95</v>
       </c>
-      <c r="AJ20">
+      <c r="AJ20" s="13">
         <v>0.94</v>
       </c>
-      <c r="AK20">
+      <c r="AK20" s="13">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="AL20">
+      <c r="AL20" s="13">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="AN20">
-        <v>0.25</v>
-      </c>
-      <c r="AO20">
-        <v>0.25</v>
-      </c>
-      <c r="AQ20">
+      <c r="AN20" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AO20" s="13">
+        <v>0.25</v>
+      </c>
+      <c r="AQ20" s="13">
         <v>100</v>
       </c>
-      <c r="AR20">
+      <c r="AR20" s="13">
         <v>15.39</v>
       </c>
-      <c r="AS20">
+      <c r="AS20" s="13">
         <v>84.61</v>
       </c>
-      <c r="AT20">
+      <c r="AT20" s="13">
         <v>1</v>
       </c>
     </row>
@@ -4358,6 +4369,14 @@
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
     </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>